<commit_message>
Back to the future - up to cafe stage
</commit_message>
<xml_diff>
--- a/BackToTheFuture/FrameCompare.xlsx
+++ b/BackToTheFuture/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\BackToTheFuture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488BE758-6323-43C3-BB28-AF0974CC2B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BE636F-6EBB-42CE-B4F0-21459BE4BA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36120" yWindow="1695" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>Place</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t>Get bowling ball</t>
+  </si>
+  <si>
+    <t>Bonus countdown start</t>
+  </si>
+  <si>
+    <t>1-2 Appears</t>
+  </si>
+  <si>
+    <t>1-3 Appears</t>
+  </si>
+  <si>
+    <t>1-4 Appears</t>
+  </si>
+  <si>
+    <t>Café Appears</t>
+  </si>
+  <si>
+    <t>1st hit</t>
+  </si>
+  <si>
+    <t>51st hit</t>
   </si>
 </sst>
 </file>
@@ -288,7 +309,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -306,7 +327,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -630,11 +650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315779BE-0457-4CD0-8DEA-0D00DE0D8921}">
-  <dimension ref="A1:F320"/>
+  <dimension ref="A1:F321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -659,7 +679,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2">
@@ -669,13 +689,13 @@
         <v>45</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D37" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D38" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="2">
@@ -691,7 +711,7 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
@@ -706,7 +726,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2">
@@ -721,7 +741,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2">
@@ -736,7 +756,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="5">
@@ -751,7 +771,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="14">
@@ -766,7 +786,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="2">
@@ -781,7 +801,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="2"/>
@@ -794,155 +814,250 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>3092</v>
+      </c>
       <c r="C11" s="2">
         <v>3093</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4433</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4434</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="14">
+        <v>4563</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4564</v>
+      </c>
+      <c r="D13" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
+        <v>4668</v>
+      </c>
+      <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3" t="str">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7354</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7355</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7426</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7427</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="14">
+        <v>7484</v>
+      </c>
+      <c r="C17" s="14">
+        <v>7485</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2">
+        <v>7589</v>
+      </c>
+      <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="str">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2">
+        <v>9787</v>
+      </c>
+      <c r="C19" s="2">
+        <v>9788</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14">
+        <v>10276</v>
+      </c>
+      <c r="D20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6" t="str">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10509</v>
+      </c>
+      <c r="C21" s="2">
+        <v>10510</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="14">
+        <v>13196</v>
+      </c>
+      <c r="C22" s="14">
+        <v>13197</v>
+      </c>
+      <c r="D22" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2">
+        <v>13364</v>
+      </c>
+      <c r="C23" s="2">
+        <v>13365</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2">
+        <v>13564</v>
+      </c>
+      <c r="C24" s="2">
+        <v>13563</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2">
+        <v>17319</v>
+      </c>
+      <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3" t="str">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2">
+        <v>17976</v>
+      </c>
+      <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3" t="str">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5">
+        <v>18252</v>
+      </c>
+      <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3" t="str">
@@ -951,7 +1066,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3" t="str">
@@ -987,25 +1102,25 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6" t="str">
+      <c r="A33" s="11"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3" t="str">
+      <c r="A34" s="12"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="str">
@@ -1014,7 +1129,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3" t="str">
@@ -1023,43 +1138,46 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2">
         <v>62463</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
@@ -1113,16 +1231,16 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
@@ -1137,16 +1255,16 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
@@ -1161,16 +1279,16 @@
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
@@ -1209,16 +1327,16 @@
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="6"/>
+      <c r="A66" s="8"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
@@ -1257,16 +1375,16 @@
       <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="6"/>
+      <c r="A74" s="8"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="8"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
@@ -1305,21 +1423,21 @@
       <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="6"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="3"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
       <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1347,19 +1465,19 @@
       <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="8"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="3"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="3"/>
@@ -1383,22 +1501,22 @@
       <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="8"/>
+      <c r="A95" s="10"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="6"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="3"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
@@ -1437,16 +1555,16 @@
       <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="9"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="6"/>
+      <c r="A104" s="8"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="8"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="3"/>
+      <c r="A105" s="9"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
@@ -1461,13 +1579,13 @@
       <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
+      <c r="A108" s="8"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="8"/>
+      <c r="A109" s="10"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="3"/>
@@ -1491,16 +1609,16 @@
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
+      <c r="A113" s="8"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="3"/>
+      <c r="A114" s="9"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="6"/>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="8"/>
@@ -1563,16 +1681,16 @@
       <c r="D124" s="3"/>
     </row>
     <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125" s="9"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="6"/>
+      <c r="A125" s="8"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="8"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="3"/>
+      <c r="A126" s="9"/>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="6"/>
     </row>
     <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>
@@ -1623,16 +1741,16 @@
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A135" s="9"/>
-      <c r="B135" s="5"/>
-      <c r="C135" s="5"/>
-      <c r="D135" s="6"/>
+      <c r="A135" s="8"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="8"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="3"/>
+      <c r="A136" s="9"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="6"/>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
@@ -1707,27 +1825,27 @@
       <c r="D148" s="3"/>
     </row>
     <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149" s="7"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
+      <c r="A149" s="8"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
       <c r="D149" s="3"/>
-      <c r="E149" s="4"/>
-      <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150" s="4"/>
-      <c r="B150" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A150" s="7"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
       <c r="D150" s="3"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
+      <c r="B151" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -1914,6 +2032,7 @@
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
+      <c r="D182" s="3"/>
     </row>
     <row r="183" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
@@ -1921,6 +2040,7 @@
       <c r="C183" s="4"/>
     </row>
     <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
     </row>
@@ -2467,6 +2587,10 @@
     <row r="320" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B320" s="4"/>
       <c r="C320" s="4"/>
+    </row>
+    <row r="321" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B321" s="4"/>
+      <c r="C321" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
back to the future - up to 4-4, 181 frames ahead of fastest known wip
</commit_message>
<xml_diff>
--- a/BackToTheFuture/FrameCompare.xlsx
+++ b/BackToTheFuture/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\BackToTheFuture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BE636F-6EBB-42CE-B4F0-21459BE4BA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DC250C-C4AA-4B99-A4A7-131DAF0693A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36120" yWindow="1695" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Place</t>
   </si>
@@ -154,6 +154,69 @@
   </si>
   <si>
     <t>51st hit</t>
+  </si>
+  <si>
+    <t>2-1 appears</t>
+  </si>
+  <si>
+    <t>2-2 appears</t>
+  </si>
+  <si>
+    <t>2-3 appears</t>
+  </si>
+  <si>
+    <t>2-4 appears</t>
+  </si>
+  <si>
+    <t>Class Room appears</t>
+  </si>
+  <si>
+    <t>3-1 Appears</t>
+  </si>
+  <si>
+    <t>Hearts = 50</t>
+  </si>
+  <si>
+    <t>Bonus countdown appears</t>
+  </si>
+  <si>
+    <t>Hearts = 10</t>
+  </si>
+  <si>
+    <t>Hearts = 20</t>
+  </si>
+  <si>
+    <t>Hearts = 30</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>3-2 Appears</t>
+  </si>
+  <si>
+    <t>3-3 Appears</t>
+  </si>
+  <si>
+    <t>3-4 Appears</t>
+  </si>
+  <si>
+    <t>Dance appears</t>
+  </si>
+  <si>
+    <t>4-1 Appears</t>
+  </si>
+  <si>
+    <t>4-2 Appears</t>
+  </si>
+  <si>
+    <t>4-3 Appears</t>
+  </si>
+  <si>
+    <t>4-4 Appears</t>
   </si>
 </sst>
 </file>
@@ -163,12 +226,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -298,37 +368,35 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
@@ -650,11 +718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315779BE-0457-4CD0-8DEA-0D00DE0D8921}">
-  <dimension ref="A1:F321"/>
+  <dimension ref="A1:I346"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -679,7 +747,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2">
@@ -689,13 +757,13 @@
         <v>45</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D38" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D63" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="2">
@@ -711,7 +779,7 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
@@ -726,7 +794,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2">
@@ -741,7 +809,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2">
@@ -756,7 +824,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="5">
@@ -771,22 +839,22 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="2">
         <v>836</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="2">
         <v>837</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="2">
@@ -801,7 +869,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="2"/>
@@ -814,7 +882,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="2">
@@ -829,7 +897,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2">
@@ -844,22 +912,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="2">
         <v>4563</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="2">
         <v>4564</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="14" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="2"/>
@@ -872,7 +940,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2">
@@ -887,7 +955,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2">
@@ -901,23 +969,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="2">
         <v>7484</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="2">
         <v>7485</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="2"/>
@@ -929,8 +997,8 @@
         <v>-</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2">
@@ -944,21 +1012,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
         <v>10276</v>
       </c>
-      <c r="D20" s="15" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="2">
@@ -972,23 +1040,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="2">
         <v>13196</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="2">
         <v>13197</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="2">
@@ -1002,8 +1070,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="2">
@@ -1017,8 +1085,8 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="2"/>
@@ -1030,8 +1098,8 @@
         <v>-</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="2"/>
@@ -1042,282 +1110,667 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="H26">
+        <v>30288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="5">
+        <v>18070</v>
+      </c>
       <c r="C27" s="5">
         <v>18252</v>
       </c>
-      <c r="D27" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="2"/>
+      <c r="D27" s="6">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H27">
+        <v>30310</v>
+      </c>
+      <c r="I27">
+        <f>H27-H26</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2">
+        <v>18431</v>
+      </c>
+      <c r="C28" s="2">
+        <v>18613</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H28">
+        <v>30333</v>
+      </c>
+      <c r="I28">
+        <f>H28-H27</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2">
+        <v>21118</v>
+      </c>
+      <c r="C29" s="2">
+        <v>21300</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H29">
+        <v>30356</v>
+      </c>
+      <c r="I29">
+        <f>H29-H28</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="2">
+        <v>21352</v>
+      </c>
+      <c r="C30" s="2">
+        <v>21534</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H30">
+        <v>30379</v>
+      </c>
+      <c r="I30">
+        <f>H30-H29</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2">
+        <v>24039</v>
+      </c>
+      <c r="C31" s="2">
+        <v>24221</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H31">
+        <v>30401</v>
+      </c>
+      <c r="I31">
+        <f>H31-H30</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2">
+        <v>24273</v>
+      </c>
+      <c r="C32" s="2">
+        <v>24455</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32">
+        <v>30424</v>
+      </c>
+      <c r="I32">
+        <f>H32-H31</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2">
+        <v>26960</v>
+      </c>
+      <c r="C33" s="2">
+        <v>27142</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33">
+        <v>30447</v>
+      </c>
+      <c r="I33">
+        <f>H33-H32</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="2">
+        <v>27194</v>
+      </c>
+      <c r="C34" s="2">
+        <v>27376</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H34">
+        <v>30470</v>
+      </c>
+      <c r="I34">
+        <f>H34-H33</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2">
+        <v>29881</v>
+      </c>
+      <c r="C35" s="2">
+        <v>30063</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H35">
+        <v>30493</v>
+      </c>
+      <c r="I35">
+        <f>H35-H34</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="2">
+        <v>30051</v>
+      </c>
+      <c r="C36" s="2">
+        <v>30233</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H36">
+        <v>30516</v>
+      </c>
+      <c r="I36">
+        <f>H36-H35</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="16">
+        <v>30723</v>
+      </c>
+      <c r="C37" s="2">
+        <v>30905</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="H37">
+        <v>30539</v>
+      </c>
+      <c r="I37">
+        <f>H37-H36</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="16">
+        <v>31183</v>
+      </c>
       <c r="C38" s="2">
-        <v>62463</v>
-      </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
+        <v>31370</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="H38">
+        <v>30561</v>
+      </c>
+      <c r="I38">
+        <f>H38-H37</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="16">
+        <v>31642</v>
+      </c>
+      <c r="C39" s="2">
+        <v>31827</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39">
+        <v>30584</v>
+      </c>
+      <c r="I39">
+        <f>H39-H38</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="2">
+        <v>32479</v>
+      </c>
+      <c r="C40" s="2">
+        <v>32663</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="G40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40">
+        <v>30608</v>
+      </c>
+      <c r="I40">
+        <f>H40-H39</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="2">
+        <v>32690</v>
+      </c>
+      <c r="C41" s="2">
+        <v>32869</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="H41">
+        <v>30630</v>
+      </c>
+      <c r="I41">
+        <f>H41-H40</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="5">
+        <v>33022</v>
+      </c>
+      <c r="C42" s="5">
+        <v>33201</v>
+      </c>
+      <c r="D42" s="6">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2">
+        <v>33383</v>
+      </c>
+      <c r="C43" s="2">
+        <v>33562</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2">
+        <v>36070</v>
+      </c>
+      <c r="C44" s="2">
+        <v>36249</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="2">
+        <v>36304</v>
+      </c>
+      <c r="C45" s="2">
+        <v>36483</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="2">
+        <v>38991</v>
+      </c>
+      <c r="C46" s="2">
+        <v>39170</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="2">
+        <v>39225</v>
+      </c>
+      <c r="C47" s="2">
+        <v>39404</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="2">
+        <v>41912</v>
+      </c>
+      <c r="C48" s="2">
+        <v>42091</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="2">
+        <v>42146</v>
+      </c>
+      <c r="C49" s="2">
+        <v>42325</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="2">
+        <v>44833</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45012</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="2">
+        <v>45002</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45181</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="5">
+        <v>48574</v>
+      </c>
+      <c r="C52" s="5">
+        <v>48753</v>
+      </c>
+      <c r="D52" s="6">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="2">
+        <v>48935</v>
+      </c>
+      <c r="C53" s="2">
+        <v>49115</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="2">
+        <v>51622</v>
+      </c>
+      <c r="C54" s="2">
+        <v>51802</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="2">
+        <v>51856</v>
+      </c>
+      <c r="C55" s="2">
+        <v>52036</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="2">
+        <v>54543</v>
+      </c>
+      <c r="C56" s="2">
+        <v>54724</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="2">
+        <v>54777</v>
+      </c>
+      <c r="C57" s="2">
+        <v>54958</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="2">
+        <v>57464</v>
+      </c>
+      <c r="C58" s="2">
+        <v>57645</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="2">
+        <v>57698</v>
+      </c>
+      <c r="C59" s="2">
+        <v>57879</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
+    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
+    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C63" s="2">
+        <v>62463</v>
+      </c>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="B64" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>2</v>
+      </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1327,16 +1780,16 @@
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="8"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="6"/>
+      <c r="A67" s="8"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
@@ -1381,16 +1834,16 @@
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="6"/>
+      <c r="A75" s="8"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
@@ -1411,10 +1864,10 @@
       <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
@@ -1429,16 +1882,16 @@
       <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="9"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="6"/>
+      <c r="A83" s="8"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="3"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
@@ -1471,10 +1924,10 @@
       <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="6"/>
+      <c r="A90" s="8"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
@@ -1483,25 +1936,25 @@
       <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="3"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
+      <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="10"/>
+      <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
+      <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="3"/>
@@ -1513,10 +1966,10 @@
       <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="9"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="6"/>
+      <c r="A97" s="8"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
@@ -1531,10 +1984,10 @@
       <c r="D99" s="3"/>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="8"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="3"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="8"/>
@@ -1561,10 +2014,10 @@
       <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="9"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="6"/>
+      <c r="A105" s="8"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
@@ -1579,15 +2032,15 @@
       <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="8"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="3"/>
+      <c r="A108" s="9"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="6"/>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
+      <c r="A109" s="8"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1615,16 +2068,16 @@
       <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="9"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="6"/>
+      <c r="A114" s="8"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="3"/>
+      <c r="A115" s="9"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="6"/>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="8"/>
@@ -1633,25 +2086,25 @@
       <c r="D116" s="3"/>
     </row>
     <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="8"/>
+      <c r="A117" s="10"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="3"/>
     </row>
     <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118" s="8"/>
+      <c r="A118" s="10"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="8"/>
+      <c r="A119" s="10"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
+      <c r="A120" s="10"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="3"/>
@@ -1663,10 +2116,10 @@
       <c r="D121" s="3"/>
     </row>
     <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="3"/>
+      <c r="A122" s="9"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="6"/>
     </row>
     <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="8"/>
@@ -1687,10 +2140,10 @@
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="9"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="6"/>
+      <c r="A126" s="8"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>
@@ -1711,10 +2164,10 @@
       <c r="D129" s="3"/>
     </row>
     <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A130" s="8"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="3"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="6"/>
     </row>
     <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="8"/>
@@ -1735,7 +2188,7 @@
       <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="8"/>
+      <c r="A134" s="10"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="3"/>
@@ -1747,10 +2200,10 @@
       <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="9"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="6"/>
+      <c r="A136" s="8"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="3"/>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
@@ -1765,10 +2218,10 @@
       <c r="D138" s="3"/>
     </row>
     <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="8"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="3"/>
+      <c r="A139" s="9"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="6"/>
     </row>
     <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="8"/>
@@ -1800,202 +2253,202 @@
       <c r="C144" s="2"/>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="8"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="8"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="8"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="8"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="8"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150" s="7"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
+    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="8"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
       <c r="D150" s="3"/>
-      <c r="E150" s="4"/>
-      <c r="F150" s="3"/>
-    </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
-      <c r="B151" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D151" s="3"/>
-    </row>
-    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A152" s="4"/>
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
+    </row>
+    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="9"/>
+      <c r="B151" s="5"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="6"/>
+    </row>
+    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="8"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
       <c r="D152" s="3"/>
     </row>
-    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A153" s="4"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
+    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="8"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
       <c r="D153" s="3"/>
     </row>
-    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A154" s="4"/>
-      <c r="B154" s="4"/>
-      <c r="C154" s="4"/>
+    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="8"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A155" s="4"/>
-      <c r="B155" s="4"/>
-      <c r="C155" s="4"/>
+    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="8"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
       <c r="D155" s="3"/>
     </row>
-    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A156" s="4"/>
-      <c r="B156" s="4"/>
-      <c r="C156" s="4"/>
+    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="8"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
       <c r="D156" s="3"/>
     </row>
-    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A157" s="4"/>
-      <c r="B157" s="4"/>
-      <c r="C157" s="4"/>
+    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="8"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
       <c r="D157" s="3"/>
     </row>
-    <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A158" s="4"/>
-      <c r="B158" s="4"/>
-      <c r="C158" s="4"/>
+    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="8"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
       <c r="D158" s="3"/>
     </row>
-    <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A159" s="4"/>
-      <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
+    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="8"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
       <c r="D159" s="3"/>
     </row>
-    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A160" s="4"/>
-      <c r="B160" s="4"/>
-      <c r="C160" s="4"/>
+    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="8"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
       <c r="D160" s="3"/>
     </row>
-    <row r="161" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A161" s="4"/>
-      <c r="B161" s="4"/>
-      <c r="C161" s="4"/>
-      <c r="D161" s="3"/>
-    </row>
-    <row r="162" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A162" s="4"/>
-      <c r="B162" s="4"/>
-      <c r="C162" s="4"/>
+    <row r="161" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="9"/>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="6"/>
+    </row>
+    <row r="162" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="8"/>
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
       <c r="D162" s="3"/>
     </row>
-    <row r="163" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A163" s="4"/>
-      <c r="B163" s="4"/>
-      <c r="C163" s="4"/>
+    <row r="163" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="8"/>
+      <c r="B163" s="2"/>
+      <c r="C163" s="2"/>
       <c r="D163" s="3"/>
     </row>
-    <row r="164" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A164" s="4"/>
-      <c r="B164" s="4"/>
-      <c r="C164" s="4"/>
+    <row r="164" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="8"/>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
       <c r="D164" s="3"/>
     </row>
-    <row r="165" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A165" s="4"/>
-      <c r="B165" s="4"/>
-      <c r="C165" s="4"/>
+    <row r="165" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="8"/>
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
       <c r="D165" s="3"/>
     </row>
-    <row r="166" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A166" s="4"/>
-      <c r="B166" s="4"/>
-      <c r="C166" s="4"/>
+    <row r="166" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="8"/>
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
       <c r="D166" s="3"/>
     </row>
-    <row r="167" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A167" s="4"/>
-      <c r="B167" s="4"/>
-      <c r="C167" s="4"/>
+    <row r="167" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="8"/>
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
       <c r="D167" s="3"/>
     </row>
-    <row r="168" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A168" s="4"/>
-      <c r="B168" s="4"/>
-      <c r="C168" s="4"/>
+    <row r="168" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="8"/>
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
       <c r="D168" s="3"/>
     </row>
-    <row r="169" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A169" s="4"/>
-      <c r="B169" s="4"/>
-      <c r="C169" s="4"/>
+    <row r="169" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A169" s="8"/>
+      <c r="B169" s="2"/>
+      <c r="C169" s="2"/>
       <c r="D169" s="3"/>
     </row>
-    <row r="170" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A170" s="4"/>
-      <c r="B170" s="4"/>
-      <c r="C170" s="4"/>
+    <row r="170" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A170" s="8"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
       <c r="D170" s="3"/>
     </row>
-    <row r="171" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A171" s="4"/>
-      <c r="B171" s="4"/>
-      <c r="C171" s="4"/>
+    <row r="171" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A171" s="8"/>
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
       <c r="D171" s="3"/>
     </row>
-    <row r="172" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A172" s="4"/>
-      <c r="B172" s="4"/>
-      <c r="C172" s="4"/>
+    <row r="172" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A172" s="8"/>
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
       <c r="D172" s="3"/>
     </row>
-    <row r="173" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A173" s="4"/>
-      <c r="B173" s="4"/>
-      <c r="C173" s="4"/>
+    <row r="173" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A173" s="8"/>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
       <c r="D173" s="3"/>
     </row>
-    <row r="174" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A174" s="4"/>
-      <c r="B174" s="4"/>
-      <c r="C174" s="4"/>
+    <row r="174" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A174" s="8"/>
+      <c r="B174" s="2"/>
+      <c r="C174" s="2"/>
       <c r="D174" s="3"/>
     </row>
-    <row r="175" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A175" s="4"/>
+    <row r="175" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A175" s="7"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="3"/>
-    </row>
-    <row r="176" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E175" s="4"/>
+      <c r="F175" s="3"/>
+    </row>
+    <row r="176" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
+      <c r="B176" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D176" s="3"/>
     </row>
     <row r="177" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2038,169 +2491,219 @@
       <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
+      <c r="D183" s="3"/>
     </row>
     <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
+      <c r="D184" s="3"/>
     </row>
     <row r="185" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A185" s="4"/>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
+      <c r="D185" s="3"/>
     </row>
     <row r="186" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A186" s="4"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
+      <c r="D186" s="3"/>
     </row>
     <row r="187" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A187" s="4"/>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
+      <c r="D187" s="3"/>
     </row>
     <row r="188" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A188" s="4"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
+      <c r="D188" s="3"/>
     </row>
     <row r="189" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A189" s="4"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
+      <c r="D189" s="3"/>
     </row>
     <row r="190" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A190" s="4"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
+      <c r="D190" s="3"/>
     </row>
     <row r="191" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A191" s="4"/>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
+      <c r="D191" s="3"/>
     </row>
     <row r="192" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A192" s="4"/>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
-    </row>
-    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A193" s="4"/>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
-    </row>
-    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A194" s="4"/>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
-    </row>
-    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A195" s="4"/>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
-    </row>
-    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A196" s="4"/>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
-    </row>
-    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A197" s="4"/>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
-    </row>
-    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A198" s="4"/>
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
-    </row>
-    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A199" s="4"/>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
-    </row>
-    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A200" s="4"/>
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
-    </row>
-    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A201" s="4"/>
       <c r="B201" s="4"/>
       <c r="C201" s="4"/>
-    </row>
-    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A202" s="4"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
-    </row>
-    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A203" s="4"/>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
-    </row>
-    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A204" s="4"/>
       <c r="B204" s="4"/>
       <c r="C204" s="4"/>
-    </row>
-    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A205" s="4"/>
       <c r="B205" s="4"/>
       <c r="C205" s="4"/>
-    </row>
-    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A206" s="4"/>
       <c r="B206" s="4"/>
       <c r="C206" s="4"/>
-    </row>
-    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A207" s="4"/>
       <c r="B207" s="4"/>
       <c r="C207" s="4"/>
-    </row>
-    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A208" s="4"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4"/>
     </row>
-    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A209" s="4"/>
       <c r="B209" s="4"/>
       <c r="C209" s="4"/>
     </row>
-    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B210" s="4"/>
       <c r="C210" s="4"/>
     </row>
-    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B211" s="4"/>
       <c r="C211" s="4"/>
     </row>
-    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B212" s="4"/>
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B213" s="4"/>
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
     </row>
-    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
     </row>
-    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B216" s="4"/>
       <c r="C216" s="4"/>
     </row>
-    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B217" s="4"/>
       <c r="C217" s="4"/>
     </row>
-    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
     </row>
-    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
     </row>
-    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B220" s="4"/>
       <c r="C220" s="4"/>
     </row>
-    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B221" s="4"/>
       <c r="C221" s="4"/>
     </row>
-    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
     </row>
-    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
     </row>
-    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B224" s="4"/>
       <c r="C224" s="4"/>
     </row>
@@ -2591,6 +3094,106 @@
     <row r="321" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
+    </row>
+    <row r="322" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B322" s="4"/>
+      <c r="C322" s="4"/>
+    </row>
+    <row r="323" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B323" s="4"/>
+      <c r="C323" s="4"/>
+    </row>
+    <row r="324" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B324" s="4"/>
+      <c r="C324" s="4"/>
+    </row>
+    <row r="325" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B325" s="4"/>
+      <c r="C325" s="4"/>
+    </row>
+    <row r="326" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B326" s="4"/>
+      <c r="C326" s="4"/>
+    </row>
+    <row r="327" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B327" s="4"/>
+      <c r="C327" s="4"/>
+    </row>
+    <row r="328" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B328" s="4"/>
+      <c r="C328" s="4"/>
+    </row>
+    <row r="329" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B329" s="4"/>
+      <c r="C329" s="4"/>
+    </row>
+    <row r="330" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B330" s="4"/>
+      <c r="C330" s="4"/>
+    </row>
+    <row r="331" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B331" s="4"/>
+      <c r="C331" s="4"/>
+    </row>
+    <row r="332" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B332" s="4"/>
+      <c r="C332" s="4"/>
+    </row>
+    <row r="333" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B333" s="4"/>
+      <c r="C333" s="4"/>
+    </row>
+    <row r="334" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B334" s="4"/>
+      <c r="C334" s="4"/>
+    </row>
+    <row r="335" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B335" s="4"/>
+      <c r="C335" s="4"/>
+    </row>
+    <row r="336" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B336" s="4"/>
+      <c r="C336" s="4"/>
+    </row>
+    <row r="337" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B337" s="4"/>
+      <c r="C337" s="4"/>
+    </row>
+    <row r="338" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B338" s="4"/>
+      <c r="C338" s="4"/>
+    </row>
+    <row r="339" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B339" s="4"/>
+      <c r="C339" s="4"/>
+    </row>
+    <row r="340" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B340" s="4"/>
+      <c r="C340" s="4"/>
+    </row>
+    <row r="341" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B341" s="4"/>
+      <c r="C341" s="4"/>
+    </row>
+    <row r="342" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B342" s="4"/>
+      <c r="C342" s="4"/>
+    </row>
+    <row r="343" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B343" s="4"/>
+      <c r="C343" s="4"/>
+    </row>
+    <row r="344" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B344" s="4"/>
+      <c r="C344" s="4"/>
+    </row>
+    <row r="345" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B345" s="4"/>
+      <c r="C345" s="4"/>
+    </row>
+    <row r="346" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B346" s="4"/>
+      <c r="C346" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2755,16 +3358,16 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="2">
         <v>5878</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="2">
         <v>5928</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -2863,7 +3466,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="2">
@@ -3134,7 +3737,7 @@
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="2"/>

</xml_diff>

<commit_message>
Back to the future done
</commit_message>
<xml_diff>
--- a/BackToTheFuture/FrameCompare.xlsx
+++ b/BackToTheFuture/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\BackToTheFuture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DC250C-C4AA-4B99-A4A7-131DAF0693A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251A00DB-ADCB-439A-A57E-2C3EA608974F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36120" yWindow="1695" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t>Place</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>4-4 Appears</t>
+  </si>
+  <si>
+    <t>Final screen appears</t>
+  </si>
+  <si>
+    <t>Cross Finish</t>
   </si>
 </sst>
 </file>
@@ -721,8 +727,8 @@
   <dimension ref="A1:I346"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1730,36 +1736,60 @@
       <c r="A60" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
+      <c r="B60" s="2">
+        <v>60385</v>
+      </c>
+      <c r="C60" s="2">
+        <v>60566</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="2">
+        <v>60617</v>
+      </c>
+      <c r="C61" s="2">
+        <v>60798</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A62" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="2">
+        <v>61808</v>
+      </c>
+      <c r="C62" s="2">
+        <v>61989</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="0"/>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="2">
+        <v>61807</v>
+      </c>
       <c r="C63" s="2">
         <v>62463</v>
       </c>
-      <c r="D63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D63" s="3">
+        <f t="shared" si="0"/>
+        <v>656</v>
       </c>
       <c r="E63" s="2"/>
     </row>

</xml_diff>